<commit_message>
fixed bug on trilateration experience
</commit_message>
<xml_diff>
--- a/FINGERPRINT/results_fingerprinting.xlsx
+++ b/FINGERPRINT/results_fingerprinting.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\5th Year College\TESE\Desenvolvimento\Code\Application\findLocationApp\findLocation\Server\Notebooks\FINGERPRINT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\College\5th Year College\TESE\Desenvolvimento\Code\Application\IPS\Notebooks\FINGERPRINT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67EDC2C-3D3F-428A-A553-3742164BE770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{ED94A9A9-2D96-408D-88F3-05CCE0EAD375}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1116" yWindow="1116" windowWidth="17280" windowHeight="8964" xr2:uid="{22682DBA-70EE-47D9-880F-69553294C7AC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{22682DBA-70EE-47D9-880F-69553294C7AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -11242,8 +11243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9805F76B-573A-4178-B9E3-1E65A92A3888}">
   <dimension ref="B2:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H88" sqref="H88"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11253,7 +11254,7 @@
     <col min="4" max="4" width="29" customWidth="1"/>
     <col min="5" max="5" width="29.44140625" customWidth="1"/>
     <col min="6" max="6" width="46.21875" customWidth="1"/>
-    <col min="7" max="7" width="35.33203125" customWidth="1"/>
+    <col min="7" max="7" width="42.109375" customWidth="1"/>
     <col min="8" max="8" width="21.5546875" customWidth="1"/>
     <col min="9" max="9" width="13.33203125" customWidth="1"/>
     <col min="10" max="10" width="15.77734375" customWidth="1"/>

</xml_diff>